<commit_message>
Update Manual Testing create_issues to add multiple assignees
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0F42A5-2FB6-874F-BCE1-EDFF6257139D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4FFE8D-CC8A-E646-B266-06A7472DAD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="8740" windowWidth="21600" windowHeight="23840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="29700" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>Manual Testing Live Data ISIS</t>
   </si>
   <si>
-    <t>Manual Testing ISIS SANS (new GUI)</t>
-  </si>
-  <si>
     <t>Manual Testing ISIS Reflectometry</t>
   </si>
   <si>
@@ -134,16 +131,7 @@
     <t>https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html</t>
   </si>
   <si>
-    <t>DannyHindson</t>
-  </si>
-  <si>
-    <t>DanielMurphy22</t>
-  </si>
-  <si>
     <t>Manual Testing Workbench Group 1- 4</t>
-  </si>
-  <si>
-    <t>RichardWaiteSTFC</t>
   </si>
   <si>
     <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
@@ -191,6 +179,18 @@
   <si>
     <t>See instructions at: https://developer.mantidproject.org/Testing/MuonAnalysis_test_guides/index.html
 https://developer.mantidproject.org/Testing/MuonInterface/MuonTesting.html</t>
+  </si>
+  <si>
+    <t>RichardWaiteSTFC, martyngigg, SilkeSchomann, sf1919, ConorMFinn</t>
+  </si>
+  <si>
+    <t>DanielMurphy22, gemmaguest, AnthonyLim23, Pasarus</t>
+  </si>
+  <si>
+    <t>DannyHindson, MialLewis, DavidFair, Harrietbrown, thomashampson</t>
+  </si>
+  <si>
+    <t>Manual Testing ISIS SANS</t>
   </si>
 </sst>
 </file>
@@ -1102,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1126,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -1134,155 +1134,155 @@
     </row>
     <row r="2" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2"/>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9"/>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1290,44 +1290,44 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Fit Script Generator testing issue
also update link for Sample Transmission calculator
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4FFE8D-CC8A-E646-B266-06A7472DAD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA1AE43-E6E0-9347-A9E3-4940799624F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="29700" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="32720" windowHeight="22900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Title</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Manual Testing Project Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Manual Testing Sliceviewer</t>
   </si>
   <si>
     <t>Manual Testing Mantid Basics Course</t>
@@ -132,10 +129,6 @@
   </si>
   <si>
     <t>Manual Testing Workbench Group 1- 4</t>
-  </si>
-  <si>
-    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
-See https://docs.mantidproject.or/interfaces/general/Sample%20Transmission%20Calculator.html</t>
   </si>
   <si>
     <t>https://docs.mantidproject.org/interfaces/utility/Filter%20Events.html</t>
@@ -191,6 +184,22 @@
   </si>
   <si>
     <t>Manual Testing ISIS SANS</t>
+  </si>
+  <si>
+    <t>Manual Testing Sliceviewer</t>
+  </si>
+  <si>
+    <t>Manual Testing Fit Script Generator</t>
+  </si>
+  <si>
+    <t>https://docs.mantidproject.org/nightly/interfaces/general/Fit%20Script%20Generator.html</t>
+  </si>
+  <si>
+    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
+See https://docs.mantidproject.org/interfaces/general/Sample%20Transmission%20Calculator.html</t>
+  </si>
+  <si>
+    <t>NEW TEST ISSUE SO PLEASE ASSIGN!!!</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1135,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -1137,11 +1146,11 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2"/>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="192" x14ac:dyDescent="0.2">
@@ -1149,23 +1158,23 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1173,10 +1182,10 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1184,11 +1193,11 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1196,11 +1205,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -1208,10 +1217,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1219,11 +1228,11 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9"/>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -1231,11 +1240,11 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1243,23 +1252,23 @@
         <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1267,22 +1276,22 @@
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1290,11 +1299,11 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1305,7 +1314,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -1316,18 +1325,29 @@
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1346,9 +1366,10 @@
     <hyperlink ref="B8" r:id="rId9" xr:uid="{224D99D6-5C3A-744B-9593-DE7284850D49}"/>
     <hyperlink ref="B16" r:id="rId10" xr:uid="{FAB9FA5C-6634-A341-95CA-A38A167549A4}"/>
     <hyperlink ref="B7" r:id="rId11" xr:uid="{09F63A2D-A77F-B444-A9B1-122002D27174}"/>
+    <hyperlink ref="B19" r:id="rId12" xr:uid="{FBFE744F-1B88-ED43-B3DA-96F45AE7857D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>

<commit_message>
Add Fit Script Generator testing issue (#105)
also update link for Sample Transmission calculator
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4FFE8D-CC8A-E646-B266-06A7472DAD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA1AE43-E6E0-9347-A9E3-4940799624F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="29700" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="32720" windowHeight="22900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Title</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Manual Testing Project Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Manual Testing Sliceviewer</t>
   </si>
   <si>
     <t>Manual Testing Mantid Basics Course</t>
@@ -132,10 +129,6 @@
   </si>
   <si>
     <t>Manual Testing Workbench Group 1- 4</t>
-  </si>
-  <si>
-    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
-See https://docs.mantidproject.or/interfaces/general/Sample%20Transmission%20Calculator.html</t>
   </si>
   <si>
     <t>https://docs.mantidproject.org/interfaces/utility/Filter%20Events.html</t>
@@ -191,6 +184,22 @@
   </si>
   <si>
     <t>Manual Testing ISIS SANS</t>
+  </si>
+  <si>
+    <t>Manual Testing Sliceviewer</t>
+  </si>
+  <si>
+    <t>Manual Testing Fit Script Generator</t>
+  </si>
+  <si>
+    <t>https://docs.mantidproject.org/nightly/interfaces/general/Fit%20Script%20Generator.html</t>
+  </si>
+  <si>
+    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
+See https://docs.mantidproject.org/interfaces/general/Sample%20Transmission%20Calculator.html</t>
+  </si>
+  <si>
+    <t>NEW TEST ISSUE SO PLEASE ASSIGN!!!</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1135,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -1137,11 +1146,11 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2"/>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="192" x14ac:dyDescent="0.2">
@@ -1149,23 +1158,23 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1173,10 +1182,10 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1184,11 +1193,11 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1196,11 +1205,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -1208,10 +1217,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1219,11 +1228,11 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9"/>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -1231,11 +1240,11 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1243,23 +1252,23 @@
         <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1267,22 +1276,22 @@
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1290,11 +1299,11 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1305,7 +1314,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -1316,18 +1325,29 @@
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1346,9 +1366,10 @@
     <hyperlink ref="B8" r:id="rId9" xr:uid="{224D99D6-5C3A-744B-9593-DE7284850D49}"/>
     <hyperlink ref="B16" r:id="rId10" xr:uid="{FAB9FA5C-6634-A341-95CA-A38A167549A4}"/>
     <hyperlink ref="B7" r:id="rId11" xr:uid="{09F63A2D-A77F-B444-A9B1-122002D27174}"/>
+    <hyperlink ref="B19" r:id="rId12" xr:uid="{FBFE744F-1B88-ED43-B3DA-96F45AE7857D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>

<commit_message>
Update ISIS Testing docs
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mantid-development\documents\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E76E6B-1F48-9E44-96C8-8DA84CECE170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="32720" windowHeight="22900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="504" windowWidth="32724" windowHeight="22896"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>Title</t>
   </si>
@@ -151,9 +150,6 @@
 * Check that the information and exercises are up to date and work in the Workbench release candidate</t>
   </si>
   <si>
-    <t>https://developer.mantidproject.org/Testing/MSlice/MSliceTestGuide.html</t>
-  </si>
-  <si>
     <t>https://developer.mantidproject.org/Testing/LiveData/LiveDataTests.html</t>
   </si>
   <si>
@@ -171,15 +167,6 @@
 https://developer.mantidproject.org/Testing/MuonInterface/MuonTesting.html</t>
   </si>
   <si>
-    <t>RichardWaiteSTFC, martyngigg, SilkeSchomann, sf1919, ConorMFinn</t>
-  </si>
-  <si>
-    <t>DanielMurphy22, gemmaguest, AnthonyLim23, Pasarus</t>
-  </si>
-  <si>
-    <t>DannyHindson, MialLewis, DavidFair, Harrietbrown, thomashampson</t>
-  </si>
-  <si>
     <t>Manual Testing ISIS SANS</t>
   </si>
   <si>
@@ -196,16 +183,34 @@
 See https://docs.mantidproject.org/interfaces/general/Sample%20Transmission%20Calculator.html</t>
   </si>
   <si>
-    <t>NEW TEST ISSUE SO PLEASE ASSIGN!!!</t>
-  </si>
-  <si>
     <t>https://developer.mantidproject.org/Testing/SANSGUI/ISISSANSGUITests.html</t>
+  </si>
+  <si>
+    <t>RichardWaiteSTFC, ConorMFinn, ajjackson, SilkeSchomann, darominski</t>
+  </si>
+  <si>
+    <t>DanielMurphy22, gemmaguest, thomashampson, MohamedAlmaki, gui-co</t>
+  </si>
+  <si>
+    <t>Harrietbrown, jhaigh0, martyngigg, robertapplin, eurydice76</t>
+  </si>
+  <si>
+    <t>sf1919, MialLewis, perenon, rbauststfc</t>
+  </si>
+  <si>
+    <t>Manual Testing ALF</t>
+  </si>
+  <si>
+    <t>https://developer.mantidproject.org/Testing/DirectInelastic/ALFViewTests.html</t>
+  </si>
+  <si>
+    <t>https://developer.mantidproject.org/Testing/DirectInelastic/MSliceTestGuide.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -700,7 +705,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -716,6 +721,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -864,23 +870,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -916,23 +905,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1108,23 +1080,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
     <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1150,10 +1122,10 @@
       </c>
       <c r="C2"/>
       <c r="D2" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="192" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1161,11 +1133,11 @@
         <v>33</v>
       </c>
       <c r="C3"/>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="D3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1174,33 +1146,33 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="D6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1208,22 +1180,22 @@
         <v>31</v>
       </c>
       <c r="C7"/>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1232,58 +1204,58 @@
       </c>
       <c r="C9"/>
       <c r="D9" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1291,22 +1263,22 @@
         <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C15"/>
-      <c r="D15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1314,10 +1286,10 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1325,60 +1297,72 @@
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="D18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B18" r:id="rId2" xr:uid="{895C170C-6F3C-3E42-B499-D3A8F7EFC683}"/>
-    <hyperlink ref="B17" r:id="rId3" xr:uid="{F17C529D-58F7-4448-ABEF-B395CCD88504}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B15" r:id="rId5" xr:uid="{6428958E-50DB-CA4B-9A04-7B9AF09A8CA3}"/>
-    <hyperlink ref="B13" r:id="rId6" xr:uid="{33EF3DE3-2897-7A47-861C-086C920A50B4}"/>
-    <hyperlink ref="B11" r:id="rId7" xr:uid="{134CEF00-B1C3-9F49-B272-1B0E39CDFCB3}"/>
-    <hyperlink ref="B8" r:id="rId8" xr:uid="{224D99D6-5C3A-744B-9593-DE7284850D49}"/>
-    <hyperlink ref="B16" r:id="rId9" xr:uid="{FAB9FA5C-6634-A341-95CA-A38A167549A4}"/>
-    <hyperlink ref="B7" r:id="rId10" xr:uid="{09F63A2D-A77F-B444-A9B1-122002D27174}"/>
-    <hyperlink ref="B19" r:id="rId11" xr:uid="{FBFE744F-1B88-ED43-B3DA-96F45AE7857D}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html"/>
+    <hyperlink ref="B18" r:id="rId2"/>
+    <hyperlink ref="B17" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B15" r:id="rId5"/>
+    <hyperlink ref="B13" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="B8" r:id="rId8"/>
+    <hyperlink ref="B16" r:id="rId9"/>
+    <hyperlink ref="B7" r:id="rId10"/>
+    <hyperlink ref="B19" r:id="rId11"/>
+    <hyperlink ref="B20" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>C19:C24</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>assignees!$A$2:$A$5</xm:f>
           </x14:formula1>
@@ -1391,19 +1375,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1411,7 +1395,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1420,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1429,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1438,7 +1422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1447,14 +1431,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
     </row>
-    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C16">
+  <sortState ref="A4:C16">
     <sortCondition descending="1" ref="B4:B27"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
Remove old muon testing link from manual testing template
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mantid-development\documents\documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-dev\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED496F0-B4CC-485E-9EA5-2B5E122ECB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="504" windowWidth="32724" windowHeight="22896"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -163,10 +166,6 @@
 https://docs.mantidproject.org/interfaces/utility/TOF%20Converter.html </t>
   </si>
   <si>
-    <t>See instructions at: https://developer.mantidproject.org/Testing/MuonAnalysis_test_guides/index.html
-https://developer.mantidproject.org/Testing/MuonInterface/MuonTesting.html</t>
-  </si>
-  <si>
     <t>Manual Testing ISIS SANS</t>
   </si>
   <si>
@@ -186,18 +185,6 @@
     <t>https://developer.mantidproject.org/Testing/SANSGUI/ISISSANSGUITests.html</t>
   </si>
   <si>
-    <t>RichardWaiteSTFC, ConorMFinn, ajjackson, SilkeSchomann, darominski</t>
-  </si>
-  <si>
-    <t>DanielMurphy22, gemmaguest, thomashampson, MohamedAlmaki, gui-co</t>
-  </si>
-  <si>
-    <t>Harrietbrown, jhaigh0, martyngigg, robertapplin, eurydice76</t>
-  </si>
-  <si>
-    <t>sf1919, MialLewis, perenon, rbauststfc</t>
-  </si>
-  <si>
     <t>Manual Testing ALF</t>
   </si>
   <si>
@@ -205,12 +192,27 @@
   </si>
   <si>
     <t>https://developer.mantidproject.org/Testing/DirectInelastic/MSliceTestGuide.html</t>
+  </si>
+  <si>
+    <t>sf1919, robertapplin, jhaigh0, MohamedAlmaki</t>
+  </si>
+  <si>
+    <t>rbauststfc, RichardWaiteSTFC, AnthonyLim23, Gui-Pereira</t>
+  </si>
+  <si>
+    <t>SilkeSchomann, ConorMFinn, jclarkeSTFC, gemmaguest</t>
+  </si>
+  <si>
+    <t>thomashampson, MialLewis, warunawickramasingha</t>
+  </si>
+  <si>
+    <t>See instructions at: https://developer.mantidproject.org/Testing/MuonAnalysis_test_guides/index.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -705,7 +707,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -722,6 +724,7 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -782,7 +785,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="assignees"/>
@@ -795,9 +798,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -835,9 +838,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -872,7 +875,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -907,7 +910,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1080,23 +1083,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="72.68359375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1015625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1015625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1015625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1121,11 +1124,11 @@
         <v>26</v>
       </c>
       <c r="C2"/>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1133,11 +1136,11 @@
         <v>33</v>
       </c>
       <c r="C3"/>
-      <c r="D3" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D3" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1145,22 +1148,22 @@
         <v>27</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1168,11 +1171,11 @@
         <v>38</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D6" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1180,22 +1183,22 @@
         <v>31</v>
       </c>
       <c r="C7"/>
-      <c r="D7" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D7" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D8" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1203,23 +1206,23 @@
         <v>32</v>
       </c>
       <c r="C9"/>
-      <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="D9" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D10" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1227,23 +1230,23 @@
         <v>36</v>
       </c>
       <c r="C11"/>
-      <c r="D11" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12"/>
-      <c r="D12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1251,118 +1254,118 @@
         <v>35</v>
       </c>
       <c r="C13"/>
-      <c r="D13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D13" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C15"/>
-      <c r="D15" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D15" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="8" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html"/>
-    <hyperlink ref="B18" r:id="rId2"/>
-    <hyperlink ref="B17" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="B15" r:id="rId5"/>
-    <hyperlink ref="B13" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B8" r:id="rId8"/>
-    <hyperlink ref="B16" r:id="rId9"/>
-    <hyperlink ref="B7" r:id="rId10"/>
-    <hyperlink ref="B19" r:id="rId11"/>
-    <hyperlink ref="B20" r:id="rId12"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>C19:C24</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>assignees!$A$2:$A$5</xm:f>
           </x14:formula1>
@@ -1375,19 +1378,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1395,7 +1398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1413,7 +1416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1431,14 +1434,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5"/>
     </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A15" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="A4:C16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C16">
     <sortCondition descending="1" ref="B4:B27"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
Remove workspace groups manual testing issue
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-dev\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED496F0-B4CC-485E-9EA5-2B5E122ECB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2730A5-823B-48AD-9EEF-693E8638C7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Title</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Manual Testing Sample Transmission calculator</t>
-  </si>
-  <si>
-    <t>Manual Testing Workspace Groups</t>
   </si>
   <si>
     <t>Manual Testing Engineering Diffraction</t>
@@ -134,10 +131,6 @@
   </si>
   <si>
     <t>https://docs.mantidproject.org/interfaces/utility/Filter%20Events.html</t>
-  </si>
-  <si>
-    <t>* Follow the examples at http://docs.mantidproject.org/concepts/WorkspaceGroup.html 
-* Ensure MantidWorkbench displays Group Workspaces correctly in the workspace tree</t>
   </si>
   <si>
     <t>Check Online Docs and the Qt-help docs built into MantidWorkbench (from the help droppdown menu)
@@ -213,7 +206,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +353,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -707,7 +706,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -724,7 +723,8 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1084,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1110,7 +1110,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -1118,222 +1118,210 @@
     </row>
     <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2"/>
       <c r="D2" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3"/>
       <c r="D3" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" t="s">
-        <v>51</v>
+      <c r="D4" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7"/>
       <c r="D7" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9"/>
-      <c r="D9" s="8" t="s">
+      <c r="B11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11" s="9" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11"/>
-      <c r="D11" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C12"/>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D12" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13"/>
-      <c r="D13" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15"/>
-      <c r="D15" s="8" t="s">
-        <v>50</v>
+        <v>3</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="D18" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1342,17 +1330,17 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B16" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B14" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B12" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B15" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
@@ -1363,13 +1351,13 @@
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C19:C24</xm:sqref>
+          <xm:sqref>C18:C23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>assignees!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C18</xm:sqref>
+          <xm:sqref>C2:C17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Update manual testing issue links
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-dev\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2730A5-823B-48AD-9EEF-693E8638C7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30FB3D7-3B92-4B63-9EAF-4A86AB77D62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>Title</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Manual Testing Documentation</t>
   </si>
   <si>
-    <t>Manual Testing ISIS Indirect interfaces</t>
-  </si>
-  <si>
     <t>Manual Testing Error Reporter</t>
   </si>
   <si>
@@ -112,10 +109,6 @@
   </si>
   <si>
     <t>Manual Testing Mantid Basics Course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Follow the directions at: https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html
-</t>
   </si>
   <si>
     <t>https://developer.mantidproject.org/Testing/Core/Core.html</t>
@@ -181,12 +174,6 @@
     <t>Manual Testing ALF</t>
   </si>
   <si>
-    <t>https://developer.mantidproject.org/Testing/DirectInelastic/ALFViewTests.html</t>
-  </si>
-  <si>
-    <t>https://developer.mantidproject.org/Testing/DirectInelastic/MSliceTestGuide.html</t>
-  </si>
-  <si>
     <t>sf1919, robertapplin, jhaigh0, MohamedAlmaki</t>
   </si>
   <si>
@@ -200,13 +187,73 @@
   </si>
   <si>
     <t>See instructions at: https://developer.mantidproject.org/Testing/MuonAnalysis_test_guides/index.html</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Follow the directions at:</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> https://developer.mantidproject.org/Testing/Indirect/DataReductionTests.html
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Follow the directions at:</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> https://developer.mantidproject.org/Testing/Inelastic/DataAnalysisTests.html https://developer.mantidproject.org/Testing/Inelastic/DataManipulationTests.html
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Manual Testing Inelastic interfaces</t>
+  </si>
+  <si>
+    <t>Manual Testing Indirect interfaces</t>
+  </si>
+  <si>
+    <t>https://developer.mantidproject.org/Testing/Direct/ALFViewTests.html</t>
+  </si>
+  <si>
+    <t>https://developer.mantidproject.org/Testing/Direct/MSliceTestGuide.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,6 +406,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -724,7 +778,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1084,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1110,174 +1164,175 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C2"/>
       <c r="D2" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C3"/>
       <c r="D3" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4"/>
+      <c r="D4" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="B6" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7"/>
-      <c r="D7" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10"/>
-      <c r="D10" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="B11" s="4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C11"/>
-      <c r="D11" s="9" t="s">
-        <v>49</v>
+      <c r="D11" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12"/>
-      <c r="D12" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14"/>
-      <c r="D14" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="B15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1285,65 +1340,77 @@
         <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="1" t="s">
+      <c r="D17" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="D19" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B16" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B14" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B12" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B15" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B2" r:id="rId13" display="https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html" xr:uid="{4DA1985E-8949-4CC1-A6D2-454A6AC9633C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1351,13 +1418,13 @@
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C18:C23</xm:sqref>
+          <xm:sqref>C19:C24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>assignees!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C17</xm:sqref>
+          <xm:sqref>C2:C18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Remove unnecessary hyperlinks from excel
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-dev\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30FB3D7-3B92-4B63-9EAF-4A86AB77D62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D2BF7A-0E54-4398-8CDC-B018FFD89D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -189,71 +189,34 @@
     <t>See instructions at: https://developer.mantidproject.org/Testing/MuonAnalysis_test_guides/index.html</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Follow the directions at:</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> https://developer.mantidproject.org/Testing/Indirect/DataReductionTests.html
+    <t>Manual Testing Inelastic interfaces</t>
+  </si>
+  <si>
+    <t>Manual Testing Indirect interfaces</t>
+  </si>
+  <si>
+    <t>https://developer.mantidproject.org/Testing/Direct/ALFViewTests.html</t>
+  </si>
+  <si>
+    <t>https://developer.mantidproject.org/Testing/Direct/MSliceTestGuide.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow the directions at:
+* https://developer.mantidproject.org/Testing/Inelastic/DataAnalysisTests.html 
+* https://developer.mantidproject.org/Testing/Inelastic/DataManipulationTests.html
 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Follow the directions at:</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> https://developer.mantidproject.org/Testing/Inelastic/DataAnalysisTests.html https://developer.mantidproject.org/Testing/Inelastic/DataManipulationTests.html
+  </si>
+  <si>
+    <t xml:space="preserve">Follow the directions at: 
+* https://developer.mantidproject.org/Testing/Indirect/DataReductionTests.html
 </t>
-    </r>
-  </si>
-  <si>
-    <t>Manual Testing Inelastic interfaces</t>
-  </si>
-  <si>
-    <t>Manual Testing Indirect interfaces</t>
-  </si>
-  <si>
-    <t>https://developer.mantidproject.org/Testing/Direct/ALFViewTests.html</t>
-  </si>
-  <si>
-    <t>https://developer.mantidproject.org/Testing/Direct/MSliceTestGuide.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,13 +369,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -760,7 +716,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -779,6 +735,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1140,20 +1099,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.68359375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1015625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1015625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1015625" style="1"/>
+    <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1170,31 +1129,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C2"/>
       <c r="D2" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C3"/>
       <c r="D3" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1206,7 +1165,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1218,7 +1177,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1229,7 +1188,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1241,7 +1200,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1253,7 +1212,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1264,7 +1223,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1276,7 +1235,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1288,7 +1247,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -1300,7 +1259,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1312,7 +1271,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1323,19 +1282,19 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15"/>
       <c r="D15" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1346,7 +1305,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -1357,7 +1316,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1368,7 +1327,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1379,12 +1338,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>42</v>
@@ -1395,22 +1354,20 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B2" r:id="rId13" display="https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html" xr:uid="{4DA1985E-8949-4CC1-A6D2-454A6AC9633C}"/>
+    <hyperlink ref="B18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B15" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B16" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B19" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B20" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1440,12 +1397,12 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1453,7 +1410,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1462,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1471,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1480,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1489,10 +1446,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
     </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix assignee page in ISIS issue template
Previously it was only counting team labels, now it counts how
many issues are assigned to each user.
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-dev\documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mantid\Clean\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D2BF7A-0E54-4398-8CDC-B018FFD89D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DA67C0-22A0-4A2C-A1F4-A23A397D96A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>Title</t>
   </si>
@@ -61,18 +61,6 @@
   </si>
   <si>
     <t>Label</t>
-  </si>
-  <si>
-    <t>ISIS Team: Core</t>
-  </si>
-  <si>
-    <t>ISIS Team: Spectroscopy</t>
-  </si>
-  <si>
-    <t>ISIS Team: Diffraction</t>
-  </si>
-  <si>
-    <t>ISIS Team: LSS</t>
   </si>
   <si>
     <t>Manual Testing M-slice</t>
@@ -174,18 +162,6 @@
     <t>Manual Testing ALF</t>
   </si>
   <si>
-    <t>sf1919, robertapplin, jhaigh0, MohamedAlmaki</t>
-  </si>
-  <si>
-    <t>rbauststfc, RichardWaiteSTFC, AnthonyLim23, Gui-Pereira</t>
-  </si>
-  <si>
-    <t>SilkeSchomann, ConorMFinn, jclarkeSTFC, gemmaguest</t>
-  </si>
-  <si>
-    <t>thomashampson, MialLewis, warunawickramasingha</t>
-  </si>
-  <si>
     <t>See instructions at: https://developer.mantidproject.org/Testing/MuonAnalysis_test_guides/index.html</t>
   </si>
   <si>
@@ -210,13 +186,55 @@
     <t xml:space="preserve">Follow the directions at: 
 * https://developer.mantidproject.org/Testing/Indirect/DataReductionTests.html
 </t>
+  </si>
+  <si>
+    <t>cailafinn, thomashampson, MohamedAlmaki, adriazalvarez</t>
+  </si>
+  <si>
+    <t>jclarkeSTFC, GuiMacielPereira, rbauststfc, warunawickramasingha</t>
+  </si>
+  <si>
+    <t>jhaigh0, SilkeSchomann, sf1919</t>
+  </si>
+  <si>
+    <t>cailafinn</t>
+  </si>
+  <si>
+    <t>thomashampson</t>
+  </si>
+  <si>
+    <t>MohamedAlmaki</t>
+  </si>
+  <si>
+    <t>adriazalvarez</t>
+  </si>
+  <si>
+    <t>jclarkeSTFC</t>
+  </si>
+  <si>
+    <t>GuiMacielPereira</t>
+  </si>
+  <si>
+    <t>rbauststfc</t>
+  </si>
+  <si>
+    <t>warunawickramasingha</t>
+  </si>
+  <si>
+    <t>jhaigh0</t>
+  </si>
+  <si>
+    <t>SilkeSchomann</t>
+  </si>
+  <si>
+    <t>sf1919</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,12 +381,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -716,7 +728,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -733,11 +745,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1099,20 +1106,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="72.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1123,230 +1130,230 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>52</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C2"/>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C15"/>
+      <c r="D15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8"/>
-      <c r="D8" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11"/>
-      <c r="D11" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12"/>
-      <c r="D12" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13"/>
-      <c r="D13" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15"/>
-      <c r="D15" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>42</v>
+      <c r="D20" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1391,18 +1398,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1410,47 +1418,115 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B2">
-        <f>COUNTIF(issues!$C:$C,assignees!A2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A2&amp;"*")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B3">
-        <f>COUNTIF(issues!$C:$C,assignees!A3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A3&amp;"*")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B4">
-        <f>COUNTIF(issues!$C:$C,assignees!A4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A4&amp;"*")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B5">
-        <f>COUNTIF(issues!$C:$C,assignees!A5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A5&amp;"*")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A6&amp;"*")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A7&amp;"*")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A8&amp;"*")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A9&amp;"*")</f>
+        <v>7</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A10&amp;"*")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A11&amp;"*")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A12&amp;"*")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
     </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
+      <c r="H15" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C16">

</xml_diff>

<commit_message>
Update link for Sample Transmission Calculator testing
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mantid\Clean\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DA67C0-22A0-4A2C-A1F4-A23A397D96A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11AA3A0-8A54-4260-9740-8F9E1D06A1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t>Title</t>
   </si>
@@ -152,10 +152,6 @@
     <t>https://docs.mantidproject.org/nightly/interfaces/general/Fit%20Script%20Generator.html</t>
   </si>
   <si>
-    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
-See https://docs.mantidproject.org/interfaces/general/Sample%20Transmission%20Calculator.html</t>
-  </si>
-  <si>
     <t>https://developer.mantidproject.org/Testing/SANSGUI/ISISSANSGUITests.html</t>
   </si>
   <si>
@@ -188,15 +184,9 @@
 </t>
   </si>
   <si>
-    <t>cailafinn, thomashampson, MohamedAlmaki, adriazalvarez</t>
-  </si>
-  <si>
     <t>jclarkeSTFC, GuiMacielPereira, rbauststfc, warunawickramasingha</t>
   </si>
   <si>
-    <t>jhaigh0, SilkeSchomann, sf1919</t>
-  </si>
-  <si>
     <t>cailafinn</t>
   </si>
   <si>
@@ -228,6 +218,22 @@
   </si>
   <si>
     <t>sf1919</t>
+  </si>
+  <si>
+    <t>eurydice76</t>
+  </si>
+  <si>
+    <t>perenon</t>
+  </si>
+  <si>
+    <t>cailafinn, jhaigh0, MohamedAlmaki, adriazalvarez</t>
+  </si>
+  <si>
+    <t>thomashampson, SilkeSchomann, sf1919, eurydice76, perenon</t>
+  </si>
+  <si>
+    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
+See https://developer.mantidproject.org/Testing/General/SampleTransmissionCalculatorTestGuide.html</t>
   </si>
 </sst>
 </file>
@@ -1104,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,7 +1125,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1136,31 +1142,32 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2"/>
       <c r="D2" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3"/>
       <c r="D3" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1169,10 +1176,10 @@
       </c>
       <c r="C4"/>
       <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1181,21 +1188,21 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1204,10 +1211,10 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1216,10 +1223,10 @@
       </c>
       <c r="C8"/>
       <c r="D8" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1227,22 +1234,22 @@
         <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1251,22 +1258,22 @@
       </c>
       <c r="C11"/>
       <c r="D11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1275,10 +1282,10 @@
       </c>
       <c r="C13"/>
       <c r="D13" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1286,22 +1293,22 @@
         <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15"/>
       <c r="D15" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1309,10 +1316,10 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1320,10 +1327,10 @@
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1331,10 +1338,10 @@
         <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1342,18 +1349,18 @@
         <v>34</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1400,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,7 +1427,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A2&amp;"*")</f>
@@ -1429,16 +1436,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A3&amp;"*")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A4&amp;"*")</f>
@@ -1447,7 +1454,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A5&amp;"*")</f>
@@ -1456,7 +1463,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A6&amp;"*")</f>
@@ -1465,7 +1472,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A7&amp;"*")</f>
@@ -1474,7 +1481,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A8&amp;"*")</f>
@@ -1483,7 +1490,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A9&amp;"*")</f>
@@ -1493,16 +1500,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A10&amp;"*")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A11&amp;"*")</f>
@@ -1511,7 +1518,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A12&amp;"*")</f>
@@ -1519,9 +1526,22 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A13&amp;"*")</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A14&amp;"*")</f>
+        <v>5</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add timings to ISIS issue templates
The issue_template_ISIS.xlsx spreadsheet now has a record of how long
each issue took for the 6.9 and/or the 6.10 releases.

I also fixed the name of the Core test, and updated the link to the
test instructions for the Filter Events test.
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-dev\documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mantid\Clean\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A806093A-E73D-450A-96D3-0B9E10587644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0DB319-BF68-4024-81EE-B821EA997593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1035" yWindow="1470" windowWidth="26340" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>Title</t>
   </si>
@@ -106,12 +106,6 @@
   </si>
   <si>
     <t>https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html</t>
-  </si>
-  <si>
-    <t>Manual Testing Workbench Group 1- 4</t>
-  </si>
-  <si>
-    <t>https://docs.mantidproject.org/interfaces/utility/Filter%20Events.html</t>
   </si>
   <si>
     <t>Check Online Docs and the Qt-help docs built into MantidWorkbench (from the help droppdown menu)
@@ -234,6 +228,21 @@
 * https://developer.mantidproject.org/Testing/Inelastic/QENSFittingTests.html 
 * https://developer.mantidproject.org/Testing/Inelastic/DataManipulationTests.html
 </t>
+  </si>
+  <si>
+    <t>6.9 (mins)</t>
+  </si>
+  <si>
+    <t>6.10 (mins)</t>
+  </si>
+  <si>
+    <t>Average time (mins)</t>
+  </si>
+  <si>
+    <t>https://developer.mantidproject.org/Testing/Utility/FilterEventsInterfaceTest.html</t>
+  </si>
+  <si>
+    <t>Manual Testing Workbench Core</t>
   </si>
 </sst>
 </file>
@@ -1110,22 +1119,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="72.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1141,174 +1150,301 @@
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2"/>
       <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="F2" s="2">
+        <f>AVERAGEIF(G2:M2, "&lt;&gt;0")</f>
+        <v>11</v>
+      </c>
+      <c r="G2" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3"/>
       <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F20" si="0">AVERAGEIF(G3:M3, "&lt;&gt;0")</f>
+        <v>30</v>
+      </c>
+      <c r="H3" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4"/>
       <c r="D4" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="H5" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>115.5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>111</v>
+      </c>
+      <c r="H6" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H7" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C8"/>
       <c r="D8" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>15</v>
+      </c>
+      <c r="H8" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="G9" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="G10" s="1">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>82.5</v>
+      </c>
+      <c r="G11" s="1">
+        <v>60</v>
+      </c>
+      <c r="H11" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="G12" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G13" s="1">
+        <v>22</v>
+      </c>
+      <c r="H13" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="G14" s="1">
+        <v>60</v>
+      </c>
+      <c r="H14" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15"/>
       <c r="D15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="G15" s="1">
+        <v>60</v>
+      </c>
+      <c r="H15" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1316,10 +1452,20 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="G16" s="1">
+        <v>50</v>
+      </c>
+      <c r="H16" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1327,46 +1473,77 @@
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="G17" s="1">
+        <v>26</v>
+      </c>
+      <c r="H17" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="H18" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G19" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="B20" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G20" s="1">
+        <v>10</v>
+      </c>
+      <c r="H20" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="B18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
@@ -1376,9 +1553,9 @@
     <hyperlink ref="B11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B16" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B19" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B20" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B19" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B8" r:id="rId11" xr:uid="{FD2B8B35-7F58-431D-9BE2-A8C7B208C97C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
@@ -1411,13 +1588,13 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1425,72 +1602,72 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A2&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A3&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A4&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A5&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A6&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A7&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A8&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A9&amp;"*")</f>
@@ -1498,45 +1675,45 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A10&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A11&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A12&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A13&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A14&amp;"*")</f>
@@ -1544,7 +1721,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="H15" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update links in manual testing issue template
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mantid\Clean\documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-dev\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0DB319-BF68-4024-81EE-B821EA997593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18976771-775D-4809-9283-C91889F5154F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1470" windowWidth="26340" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -167,82 +167,84 @@
     <t>https://developer.mantidproject.org/Testing/Direct/MSliceTestGuide.html</t>
   </si>
   <si>
+    <t>jclarkeSTFC, GuiMacielPereira, rbauststfc, warunawickramasingha</t>
+  </si>
+  <si>
+    <t>cailafinn</t>
+  </si>
+  <si>
+    <t>thomashampson</t>
+  </si>
+  <si>
+    <t>MohamedAlmaki</t>
+  </si>
+  <si>
+    <t>adriazalvarez</t>
+  </si>
+  <si>
+    <t>jclarkeSTFC</t>
+  </si>
+  <si>
+    <t>GuiMacielPereira</t>
+  </si>
+  <si>
+    <t>rbauststfc</t>
+  </si>
+  <si>
+    <t>warunawickramasingha</t>
+  </si>
+  <si>
+    <t>jhaigh0</t>
+  </si>
+  <si>
+    <t>SilkeSchomann</t>
+  </si>
+  <si>
+    <t>sf1919</t>
+  </si>
+  <si>
+    <t>eurydice76</t>
+  </si>
+  <si>
+    <t>perenon</t>
+  </si>
+  <si>
+    <t>cailafinn, jhaigh0, MohamedAlmaki, adriazalvarez</t>
+  </si>
+  <si>
+    <t>thomashampson, SilkeSchomann, sf1919, eurydice76, perenon</t>
+  </si>
+  <si>
+    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
+See https://developer.mantidproject.org/Testing/General/SampleTransmissionCalculatorTestGuide.html</t>
+  </si>
+  <si>
+    <t>6.9 (mins)</t>
+  </si>
+  <si>
+    <t>6.10 (mins)</t>
+  </si>
+  <si>
+    <t>Average time (mins)</t>
+  </si>
+  <si>
+    <t>https://developer.mantidproject.org/Testing/Utility/FilterEventsInterfaceTest.html</t>
+  </si>
+  <si>
+    <t>Manual Testing Workbench Core</t>
+  </si>
+  <si>
     <t xml:space="preserve">Follow the directions at: 
+* https://developer.mantidproject.org/Testing/Indirect/DiffractionTests.html
 * https://developer.mantidproject.org/Testing/Indirect/DataReductionTests.html
 </t>
   </si>
   <si>
-    <t>jclarkeSTFC, GuiMacielPereira, rbauststfc, warunawickramasingha</t>
-  </si>
-  <si>
-    <t>cailafinn</t>
-  </si>
-  <si>
-    <t>thomashampson</t>
-  </si>
-  <si>
-    <t>MohamedAlmaki</t>
-  </si>
-  <si>
-    <t>adriazalvarez</t>
-  </si>
-  <si>
-    <t>jclarkeSTFC</t>
-  </si>
-  <si>
-    <t>GuiMacielPereira</t>
-  </si>
-  <si>
-    <t>rbauststfc</t>
-  </si>
-  <si>
-    <t>warunawickramasingha</t>
-  </si>
-  <si>
-    <t>jhaigh0</t>
-  </si>
-  <si>
-    <t>SilkeSchomann</t>
-  </si>
-  <si>
-    <t>sf1919</t>
-  </si>
-  <si>
-    <t>eurydice76</t>
-  </si>
-  <si>
-    <t>perenon</t>
-  </si>
-  <si>
-    <t>cailafinn, jhaigh0, MohamedAlmaki, adriazalvarez</t>
-  </si>
-  <si>
-    <t>thomashampson, SilkeSchomann, sf1919, eurydice76, perenon</t>
-  </si>
-  <si>
-    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
-See https://developer.mantidproject.org/Testing/General/SampleTransmissionCalculatorTestGuide.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">Follow the directions at:
+* https://developer.mantidproject.org/Testing/Inelastic/BayesFittingTests.html
 * https://developer.mantidproject.org/Testing/Inelastic/QENSFittingTests.html 
-* https://developer.mantidproject.org/Testing/Inelastic/DataManipulationTests.html
+* https://developer.mantidproject.org/Testing/Inelastic/DataProcessorTests.html
 </t>
-  </si>
-  <si>
-    <t>6.9 (mins)</t>
-  </si>
-  <si>
-    <t>6.10 (mins)</t>
-  </si>
-  <si>
-    <t>Average time (mins)</t>
-  </si>
-  <si>
-    <t>https://developer.mantidproject.org/Testing/Utility/FilterEventsInterfaceTest.html</t>
-  </si>
-  <si>
-    <t>Manual Testing Workbench Core</t>
   </si>
 </sst>
 </file>
@@ -1121,20 +1123,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1151,25 +1153,25 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C2"/>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="2">
         <f>AVERAGEIF(G2:M2, "&lt;&gt;0")</f>
@@ -1179,16 +1181,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C3"/>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ref="F3:F20" si="0">AVERAGEIF(G3:M3, "&lt;&gt;0")</f>
@@ -1198,7 +1200,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1207,7 +1209,7 @@
       </c>
       <c r="C4"/>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
@@ -1217,16 +1219,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
@@ -1236,7 +1238,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1244,7 +1246,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
@@ -1257,7 +1259,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1266,7 +1268,7 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
@@ -1276,16 +1278,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8"/>
       <c r="D8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
@@ -1298,7 +1300,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1306,7 +1308,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
@@ -1316,16 +1318,16 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
@@ -1338,7 +1340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1347,7 +1349,7 @@
       </c>
       <c r="C11"/>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
@@ -1360,7 +1362,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1369,7 +1371,7 @@
       </c>
       <c r="C12"/>
       <c r="D12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
@@ -1379,7 +1381,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1388,7 +1390,7 @@
       </c>
       <c r="C13"/>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
@@ -1401,7 +1403,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1409,7 +1411,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
@@ -1422,7 +1424,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1431,7 +1433,7 @@
       </c>
       <c r="C15"/>
       <c r="D15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
@@ -1444,7 +1446,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1452,7 +1454,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
@@ -1465,7 +1467,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1473,7 +1475,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="0"/>
@@ -1486,7 +1488,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1494,7 +1496,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
@@ -1504,7 +1506,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1512,7 +1514,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="0"/>
@@ -1522,7 +1524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
@@ -1530,7 +1532,7 @@
         <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="0"/>
@@ -1588,13 +1590,13 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1602,72 +1604,72 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A2&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A3&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A4&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A5&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A6&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A7&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A8&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A9&amp;"*")</f>
@@ -1675,45 +1677,45 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A10&amp;"*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A11&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A12&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A13&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A14&amp;"*")</f>
@@ -1721,7 +1723,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="H15" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add Inelastic corrections manual testing instruction link
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-dev\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18976771-775D-4809-9283-C91889F5154F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7CD7E4-47DB-43DB-B666-5CF122A0CA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -242,6 +242,7 @@
   <si>
     <t xml:space="preserve">Follow the directions at:
 * https://developer.mantidproject.org/Testing/Inelastic/BayesFittingTests.html
+* https://developer.mantidproject.org/Testing/Inelastic/CorrectionsTests.html
 * https://developer.mantidproject.org/Testing/Inelastic/QENSFittingTests.html 
 * https://developer.mantidproject.org/Testing/Inelastic/DataProcessorTests.html
 </t>
@@ -1124,7 +1125,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1181,7 +1182,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Update tests times estimate for 6.11 release
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-dev\documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy22959\Development\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7CD7E4-47DB-43DB-B666-5CF122A0CA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB8F7D7-FEE7-4EB9-A012-B5F22A4F5757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="4536" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
   <si>
     <t>Title</t>
   </si>
@@ -167,15 +167,9 @@
     <t>https://developer.mantidproject.org/Testing/Direct/MSliceTestGuide.html</t>
   </si>
   <si>
-    <t>jclarkeSTFC, GuiMacielPereira, rbauststfc, warunawickramasingha</t>
-  </si>
-  <si>
     <t>cailafinn</t>
   </si>
   <si>
-    <t>thomashampson</t>
-  </si>
-  <si>
     <t>MohamedAlmaki</t>
   </si>
   <si>
@@ -201,18 +195,6 @@
   </si>
   <si>
     <t>sf1919</t>
-  </si>
-  <si>
-    <t>eurydice76</t>
-  </si>
-  <si>
-    <t>perenon</t>
-  </si>
-  <si>
-    <t>cailafinn, jhaigh0, MohamedAlmaki, adriazalvarez</t>
-  </si>
-  <si>
-    <t>thomashampson, SilkeSchomann, sf1919, eurydice76, perenon</t>
   </si>
   <si>
     <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
@@ -247,12 +229,42 @@
 * https://developer.mantidproject.org/Testing/Inelastic/DataProcessorTests.html
 </t>
   </si>
+  <si>
+    <t>Despiix</t>
+  </si>
+  <si>
+    <t>yusufjimoh</t>
+  </si>
+  <si>
+    <t>robertapplin</t>
+  </si>
+  <si>
+    <t>RabiyaF</t>
+  </si>
+  <si>
+    <t>RichardWaiteSTFC</t>
+  </si>
+  <si>
+    <t>SilkeSchomann, robertapplin, rbauststfc</t>
+  </si>
+  <si>
+    <t>cailafinn, yusufjimoh, warunawickramasingha, sf1919</t>
+  </si>
+  <si>
+    <t>MohamedAlmaki, adriazalvarez, RichardWaiteSTFC, RabiyaF</t>
+  </si>
+  <si>
+    <t>GuiMacielPereira, jhaigh0, Despiix, jclarkeSTFC</t>
+  </si>
+  <si>
+    <t>6.11 (mins)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,13 +404,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -746,7 +751,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -761,7 +766,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
@@ -1122,22 +1126,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="72.68359375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1015625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1015625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1015625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1154,54 +1158,63 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C2"/>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F2" s="2">
         <f>AVERAGEIF(G2:M2, "&lt;&gt;0")</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G2" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="I2" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C3"/>
       <c r="D3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ref="F3:F20" si="0">AVERAGEIF(G3:M3, "&lt;&gt;0")</f>
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="H3" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="I3" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1210,7 +1223,7 @@
       </c>
       <c r="C4"/>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
@@ -1220,26 +1233,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>102.5</v>
       </c>
       <c r="H5" s="1">
         <v>120</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I5" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1247,11 +1263,11 @@
         <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>115.5</v>
+        <v>127</v>
       </c>
       <c r="G6" s="1">
         <v>111</v>
@@ -1259,8 +1275,11 @@
       <c r="H6" s="1">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I6" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1269,30 +1288,33 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="H7" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I7" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C8"/>
       <c r="D8" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1">
         <v>15</v>
@@ -1300,8 +1322,11 @@
       <c r="H8" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I8" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1309,30 +1334,33 @@
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>127.5</v>
       </c>
       <c r="G9" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="I9" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>17.5</v>
+        <v>18.333333333333332</v>
       </c>
       <c r="G10" s="1">
         <v>25</v>
@@ -1340,8 +1368,11 @@
       <c r="H10" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I10" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1350,11 +1381,11 @@
       </c>
       <c r="C11"/>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>82.5</v>
+        <v>85</v>
       </c>
       <c r="G11" s="1">
         <v>60</v>
@@ -1362,8 +1393,11 @@
       <c r="H11" s="1">
         <v>105</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I11" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1372,17 +1406,20 @@
       </c>
       <c r="C12"/>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G12" s="1">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I12" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1391,11 +1428,11 @@
       </c>
       <c r="C13"/>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20.666666666666668</v>
       </c>
       <c r="G13" s="1">
         <v>22</v>
@@ -1403,8 +1440,11 @@
       <c r="H13" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="I13" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1412,11 +1452,11 @@
         <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>53.333333333333336</v>
       </c>
       <c r="G14" s="1">
         <v>60</v>
@@ -1424,8 +1464,11 @@
       <c r="H14" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I14" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1434,11 +1477,11 @@
       </c>
       <c r="C15"/>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>56.666666666666664</v>
       </c>
       <c r="G15" s="1">
         <v>60</v>
@@ -1446,8 +1489,11 @@
       <c r="H15" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I15" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1455,11 +1501,11 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>38.666666666666664</v>
       </c>
       <c r="G16" s="1">
         <v>50</v>
@@ -1467,8 +1513,11 @@
       <c r="H16" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I16" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1476,11 +1525,11 @@
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>25.333333333333332</v>
       </c>
       <c r="G17" s="1">
         <v>26</v>
@@ -1488,8 +1537,11 @@
       <c r="H17" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I17" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1497,7 +1549,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
@@ -1507,7 +1559,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1515,35 +1567,41 @@
         <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="G19" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I19" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>15.666666666666666</v>
       </c>
       <c r="G20" s="1">
         <v>10</v>
       </c>
       <c r="H20" s="1">
         <v>20</v>
+      </c>
+      <c r="I20" s="1">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1573,7 +1631,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
-            <xm:f>assignees!$A$2:$A$5</xm:f>
+            <xm:f>assignees!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C18</xm:sqref>
         </x14:dataValidation>
@@ -1585,19 +1643,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1015625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1605,132 +1663,125 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A2&amp;"*")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A3&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A4&amp;"*")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A5&amp;"*")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A6&amp;"*")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A7&amp;"*")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A8&amp;"*")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A9&amp;"*")</f>
-        <v>7</v>
-      </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A10&amp;"*")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A11&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12">
-        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A12&amp;"*")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13">
-        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A13&amp;"*")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14">
-        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A14&amp;"*")</f>
-        <v>5</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="H15" s="1"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C16">
-    <sortCondition descending="1" ref="B4:B27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C12">
+    <sortCondition descending="1" ref="B3:B23"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
update test times for v6.12
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy22959\Development\documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB8F7D7-FEE7-4EB9-A012-B5F22A4F5757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683FBFB1-B75D-48B0-83F3-345126E2A9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="4536" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="181" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
   <si>
     <t>Title</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>http://developer.mantidproject.org/Testing/ErrorReporter-ProjectRecovery/ErrorReporterTesting.html</t>
-  </si>
-  <si>
-    <t>size</t>
   </si>
   <si>
     <t>No Assigned</t>
@@ -201,9 +198,6 @@
 See https://developer.mantidproject.org/Testing/General/SampleTransmissionCalculatorTestGuide.html</t>
   </si>
   <si>
-    <t>6.9 (mins)</t>
-  </si>
-  <si>
     <t>6.10 (mins)</t>
   </si>
   <si>
@@ -239,32 +233,89 @@
     <t>robertapplin</t>
   </si>
   <si>
-    <t>RabiyaF</t>
-  </si>
-  <si>
     <t>RichardWaiteSTFC</t>
   </si>
   <si>
-    <t>SilkeSchomann, robertapplin, rbauststfc</t>
-  </si>
-  <si>
-    <t>cailafinn, yusufjimoh, warunawickramasingha, sf1919</t>
-  </si>
-  <si>
-    <t>MohamedAlmaki, adriazalvarez, RichardWaiteSTFC, RabiyaF</t>
-  </si>
-  <si>
-    <t>GuiMacielPereira, jhaigh0, Despiix, jclarkeSTFC</t>
-  </si>
-  <si>
     <t>6.11 (mins)</t>
+  </si>
+  <si>
+    <t>andy-bridger</t>
+  </si>
+  <si>
+    <t>MialLewis</t>
+  </si>
+  <si>
+    <t>Group 1: James(OSX)*, Gui(linux), Jonathan(IDaaS), Despina(Windows)</t>
+  </si>
+  <si>
+    <t>total time</t>
+  </si>
+  <si>
+    <t>jclarkeSTFC, GuiMacielPereira, jhaigh0, Despiix</t>
+  </si>
+  <si>
+    <t>rbauststfc, adriazalvarez, MohamedAlmaki, MialLewis</t>
+  </si>
+  <si>
+    <t>RichardWaiteSTFC, yusufjimoh, SilkeSchomann, andy-bridger</t>
+  </si>
+  <si>
+    <t>Gui</t>
+  </si>
+  <si>
+    <t>Waruna</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>Silke</t>
+  </si>
+  <si>
+    <t>Conda</t>
+  </si>
+  <si>
+    <t>GPU IDAaaS</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Group 4: Richard(IDAaaS)*, Yusuf(linux), Silke(OSX), Andy(Windows)</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thomashampson </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cailafinn, warunawickramasingha, robertapplin, thomashampson </t>
+  </si>
+  <si>
+    <t>cailafinn, warunawickramasingha, robertapplin, thomashampson</t>
+  </si>
+  <si>
+    <t>Group 2: Caila(OSX)*, Waruna(IDaaS), Rob(linux), Tom(Windows)</t>
+  </si>
+  <si>
+    <t>Group 3: Rachel(IDAaaS)*, Adrian(Windows), Mohammed(linux), Mial(OSX), ILL(linux)</t>
+  </si>
+  <si>
+    <t>6.12 (mints)</t>
+  </si>
+  <si>
+    <t>6.9  (mins)</t>
+  </si>
+  <si>
+    <t>6.13 (mints)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +458,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -751,7 +808,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -767,6 +824,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1126,22 +1185,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.68359375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1015625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1015625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1015625" style="1"/>
+    <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1149,459 +1208,501 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>82</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2"/>
       <c r="D2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="2">
-        <f>AVERAGEIF(G2:M2, "&lt;&gt;0")</f>
-        <v>28</v>
-      </c>
-      <c r="G2" s="1">
+        <v>65</v>
+      </c>
+      <c r="E2" s="2">
+        <f>AVERAGEIF(F2:L2, "&lt;&gt;0")</f>
+        <v>23.666666666666668</v>
+      </c>
+      <c r="F2" s="1">
         <v>11</v>
       </c>
+      <c r="H2" s="2">
+        <v>45</v>
+      </c>
       <c r="I2" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3"/>
       <c r="D3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="2">
-        <f t="shared" ref="F3:F20" si="0">AVERAGEIF(G3:M3, "&lt;&gt;0")</f>
+        <v>66</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E20" si="0">AVERAGEIF(F3:L3, "&lt;&gt;0")</f>
         <v>70</v>
       </c>
+      <c r="G3" s="1">
+        <v>30</v>
+      </c>
       <c r="H3" s="1">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4"/>
       <c r="D4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="2">
+        <v>78</v>
+      </c>
+      <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H4" s="1">
+      <c r="G4" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="2">
+        <v>65</v>
+      </c>
+      <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>102.5</v>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="G5" s="1">
+        <v>120</v>
       </c>
       <c r="H5" s="1">
+        <v>85</v>
+      </c>
+      <c r="I5" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>125.25</v>
+      </c>
+      <c r="F6" s="1">
+        <v>111</v>
+      </c>
+      <c r="G6" s="1">
         <v>120</v>
       </c>
-      <c r="I5" s="1">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" si="0"/>
-        <v>127</v>
-      </c>
-      <c r="G6" s="1">
-        <v>111</v>
-      </c>
       <c r="H6" s="1">
+        <v>150</v>
+      </c>
+      <c r="I6" s="1">
         <v>120</v>
       </c>
-      <c r="I6" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="2">
+        <v>67</v>
+      </c>
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>12.5</v>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="G7" s="1">
+        <v>10</v>
       </c>
       <c r="H7" s="1">
+        <v>15</v>
+      </c>
+      <c r="I7" s="1">
         <v>10</v>
       </c>
-      <c r="I7" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8"/>
       <c r="D8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="2">
+        <v>67</v>
+      </c>
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18.75</v>
+      </c>
+      <c r="F8" s="1">
+        <v>15</v>
       </c>
       <c r="G8" s="1">
+        <v>30</v>
+      </c>
+      <c r="H8" s="1">
         <v>15</v>
-      </c>
-      <c r="H8" s="1">
-        <v>30</v>
       </c>
       <c r="I8" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="2">
+        <v>79</v>
+      </c>
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>127.5</v>
       </c>
-      <c r="G9" s="1">
+      <c r="F9" s="1">
         <v>150</v>
       </c>
-      <c r="I9" s="1">
+      <c r="H9" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="2">
+        <v>79</v>
+      </c>
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>18.333333333333332</v>
+        <v>19</v>
+      </c>
+      <c r="F10" s="1">
+        <v>25</v>
       </c>
       <c r="G10" s="1">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1">
+        <v>20</v>
+      </c>
+      <c r="I10" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="H10" s="1">
-        <v>10</v>
-      </c>
-      <c r="I10" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="2">
+        <v>67</v>
+      </c>
+      <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>78.75</v>
+      </c>
+      <c r="F11" s="1">
+        <v>60</v>
       </c>
       <c r="G11" s="1">
+        <v>105</v>
+      </c>
+      <c r="H11" s="1">
+        <v>90</v>
+      </c>
+      <c r="I11" s="1">
         <v>60</v>
       </c>
-      <c r="H11" s="1">
-        <v>105</v>
-      </c>
-      <c r="I11" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="2">
+        <v>65</v>
+      </c>
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="G12" s="1">
+        <v>63.333333333333336</v>
+      </c>
+      <c r="F12" s="1">
         <v>67</v>
       </c>
+      <c r="H12" s="1">
+        <v>53</v>
+      </c>
       <c r="I12" s="1">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="2">
+        <v>79</v>
+      </c>
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>20.666666666666668</v>
+        <v>26.5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>22</v>
       </c>
       <c r="G13" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H13" s="1">
         <v>20</v>
       </c>
       <c r="I13" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="2">
+        <v>66</v>
+      </c>
+      <c r="E14" s="2">
         <f t="shared" si="0"/>
         <v>53.333333333333336</v>
       </c>
+      <c r="F14" s="1">
+        <v>60</v>
+      </c>
       <c r="G14" s="1">
+        <v>40</v>
+      </c>
+      <c r="H14" s="1">
         <v>60</v>
       </c>
-      <c r="H14" s="1">
-        <v>40</v>
-      </c>
-      <c r="I14" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15"/>
       <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="2">
+        <v>79</v>
+      </c>
+      <c r="E15" s="2">
         <f t="shared" si="0"/>
         <v>56.666666666666664</v>
       </c>
+      <c r="F15" s="1">
+        <v>60</v>
+      </c>
       <c r="G15" s="1">
         <v>60</v>
       </c>
       <c r="H15" s="1">
-        <v>60</v>
-      </c>
-      <c r="I15" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="2">
+        <v>65</v>
+      </c>
+      <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>38.666666666666664</v>
+        <v>40.25</v>
+      </c>
+      <c r="F16" s="1">
+        <v>50</v>
       </c>
       <c r="G16" s="1">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H16" s="1">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I16" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="2">
+        <v>67</v>
+      </c>
+      <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>25.333333333333332</v>
+        <v>24</v>
+      </c>
+      <c r="F17" s="1">
+        <v>26</v>
       </c>
       <c r="G17" s="1">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H17" s="1">
+        <v>30</v>
+      </c>
+      <c r="I17" s="1">
         <v>20</v>
       </c>
-      <c r="I17" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="2">
+        <v>66</v>
+      </c>
+      <c r="E18" s="2">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="H18" s="1">
+      <c r="G18" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="D19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="2">
+        <v>66</v>
+      </c>
+      <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>12.5</v>
-      </c>
-      <c r="G19" s="1">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="F19" s="1">
         <v>10</v>
+      </c>
+      <c r="H19" s="1">
+        <v>15</v>
       </c>
       <c r="I19" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="2">
+        <v>65</v>
+      </c>
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
-        <v>15.666666666666666</v>
+        <v>15.5</v>
+      </c>
+      <c r="F20" s="1">
+        <v>10</v>
       </c>
       <c r="G20" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H20" s="1">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I20" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1622,7 +1723,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
@@ -1643,83 +1744,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="81.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A2&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A3&amp;"*")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A4&amp;"*")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A5&amp;"*")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A6&amp;"*")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A7&amp;"*")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A8&amp;"*")</f>
@@ -1727,57 +1832,237 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A9&amp;"*")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A10&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11">
         <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A11&amp;"*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A12&amp;"*")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A13&amp;"*")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A14&amp;"*")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A15&amp;"*")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
+      <c r="B16">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A16&amp;"*")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
+      <c r="B17">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A17&amp;"*")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18">
+        <f>COUNTIF(issues!$D$2:$D$20,"*"&amp;A18&amp;"*")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K20" t="s">
+        <v>73</v>
+      </c>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="F21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21">
+        <v>243</v>
+      </c>
+      <c r="I21">
+        <f>H21-$H$25</f>
+        <v>-16.5</v>
+      </c>
+      <c r="J21" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" t="s">
+        <v>76</v>
+      </c>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="F22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22">
+        <f>223+18</f>
+        <v>241</v>
+      </c>
+      <c r="I22">
+        <f>H22-$H$25</f>
+        <v>-18.5</v>
+      </c>
+      <c r="J22" t="s">
+        <v>69</v>
+      </c>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="F23" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23">
+        <f>303-18</f>
+        <v>285</v>
+      </c>
+      <c r="I23">
+        <f>H23-$H$25</f>
+        <v>25.5</v>
+      </c>
+      <c r="J23" t="s">
+        <v>70</v>
+      </c>
+      <c r="K23" t="s">
+        <v>74</v>
+      </c>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="F24" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24">
+        <v>269</v>
+      </c>
+      <c r="I24">
+        <f>H24-$H$25</f>
+        <v>9.5</v>
+      </c>
+      <c r="J24" t="s">
+        <v>71</v>
+      </c>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H25" s="8">
+        <f>AVERAGE(H21:H24)</f>
+        <v>259.5</v>
+      </c>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M36" s="1"/>
+    </row>
+    <row r="37" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M38" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C12">

</xml_diff>

<commit_message>
update script and issue template
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2AAE72-B345-4E0D-8AE6-25E267B96540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68514852-FF34-4380-85F6-926DC3A23F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4815" windowWidth="29040" windowHeight="15720" tabRatio="169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">issues!$A$1:$K$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">issues!$A$1:$L$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
   <si>
     <t>Title</t>
   </si>
@@ -191,9 +191,6 @@
     <t>SilkeSchomann</t>
   </si>
   <si>
-    <t>sf1919</t>
-  </si>
-  <si>
     <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
 See https://developer.mantidproject.org/Testing/General/SampleTransmissionCalculatorTestGuide.html</t>
   </si>
@@ -230,9 +227,6 @@
     <t>MialLewis</t>
   </si>
   <si>
-    <t xml:space="preserve">thomashampson </t>
-  </si>
-  <si>
     <t>6.12 (mints)</t>
   </si>
   <si>
@@ -242,20 +236,41 @@
     <t>6.13 (mints)</t>
   </si>
   <si>
-    <t>JackEAllen</t>
-  </si>
-  <si>
     <t>v6.13 Groups</t>
   </si>
   <si>
-    <t>Group 1: Gui(linux*), Jonathan(IDaaS), Caila(OSX)*, Tom(Windows*)</t>
-  </si>
-  <si>
-    <t>Group 2: Silke(IDAaaS+), Waruna(Windows), James(OSX)*, Adrian(Windows*)</t>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>Manual Test Mantid Plotting</t>
+  </si>
+  <si>
+    <t>Make sure the Mantid Plotting is working correctly and each testing team follows below test instructions on separate test issues https://docs.mantidproject.org/nightly/tutorials/python_in_mantid/plotting/index.html</t>
+  </si>
+  <si>
+    <t>Goup name</t>
+  </si>
+  <si>
+    <t>Group members</t>
+  </si>
+  <si>
+    <t>Group 2: James(IDAaaS+), Waruna(Windows), Silke(OSX), Adrian(Windows*)</t>
+  </si>
+  <si>
+    <t>Group 1: Andy(IDAaaS), Jonathan(linux*), Mial(OSX), Tom(Windows*)</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Group 3: Mohammed(linux), Mial(OSX), Sarah(IDAaaS), </t>
+      <t xml:space="preserve">Group 3: Gui(linux), Caila(OSX)*, Richard(IDAaaS), </t>
     </r>
     <r>
       <rPr>
@@ -265,41 +280,38 @@
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
-      <t>Jack(Windows*)</t>
+      <t>Mohammed(Windows*)</t>
     </r>
   </si>
   <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GuiMacielPereira, jhaigh0, cailafinn, thomashampson </t>
-  </si>
-  <si>
-    <t>SilkeSchomann, warunawickramasingha, jclarkeSTFC, adriazalvarez</t>
-  </si>
-  <si>
-    <t>MohamedAlmaki, MialLewis, sf1919</t>
-  </si>
-  <si>
-    <t>Manual Test Mantid Plotting</t>
-  </si>
-  <si>
-    <t>Make sure the Mantid Plotting is working correctly and each testing team follows below test instructions on separate test issues https://docs.mantidproject.org/nightly/tutorials/python_in_mantid/plotting/index.html</t>
-  </si>
-  <si>
-    <t>Goup name</t>
-  </si>
-  <si>
-    <t>Group members</t>
+    <t>jclarkeSTFC, warunawickramasingha, SilkeSchomann, adriazalvarez</t>
+  </si>
+  <si>
+    <t>MohamedAlmaki, cailafinn, GuiMacielPereira, RichardWaiteSTFC</t>
+  </si>
+  <si>
+    <t>jhaigh0, MialLewis, thomashampson, andy-bridger</t>
+  </si>
+  <si>
+    <t>RichardWaiteSTFC</t>
+  </si>
+  <si>
+    <t>andy-bridger</t>
+  </si>
+  <si>
+    <t>thomashampson</t>
+  </si>
+  <si>
+    <t>Set 1</t>
+  </si>
+  <si>
+    <t>Set 2</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>Set 3</t>
   </si>
 </sst>
 </file>
@@ -826,7 +838,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -853,7 +865,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1217,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1228,12 +1239,13 @@
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
     <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="54.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="4" max="4" width="5.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="1" customWidth="1"/>
+    <col min="6" max="6" width="54.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1244,31 +1256,34 @@
         <v>6</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="G1" s="10" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -1276,122 +1291,138 @@
         <v>21</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <f>VLOOKUP(D2,assignees!$G$2:$H$4,2,0)</f>
-        <v xml:space="preserve">GuiMacielPereira, jhaigh0, cailafinn, thomashampson </v>
-      </c>
-      <c r="F2" s="2">
-        <f t="shared" ref="F2:F20" si="0">AVERAGEIF(G2:M2, "&lt;&gt;0")</f>
+      <c r="D2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="str">
+        <f>VLOOKUP(D2,assignees!$F$6:$G$8,2,0)</f>
+        <v>G1</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>VLOOKUP(E2,assignees!$G$2:$H$4,2,0)</f>
+        <v>jhaigh0, MialLewis, thomashampson, andy-bridger</v>
+      </c>
+      <c r="G2" s="2">
+        <f t="shared" ref="G2:G20" si="0">AVERAGEIF(H2:N2, "&lt;&gt;0")</f>
         <v>120</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1">
         <v>150</v>
       </c>
-      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <f>VLOOKUP(D3,assignees!$G$2:$H$4,2,0)</f>
-        <v>SilkeSchomann, warunawickramasingha, jclarkeSTFC, adriazalvarez</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="D3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="str">
+        <f>VLOOKUP(D3,assignees!$F$6:$G$8,2,0)</f>
+        <v>G3</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f>VLOOKUP(E3,assignees!$G$2:$H$4,2,0)</f>
+        <v>MohamedAlmaki, cailafinn, GuiMacielPereira, RichardWaiteSTFC</v>
+      </c>
+      <c r="G3" s="2">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>150</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>105</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="1" t="str">
-        <f>VLOOKUP(D4,assignees!$G$2:$H$4,2,0)</f>
-        <v>MohamedAlmaki, MialLewis, sf1919</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="D4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="str">
+        <f>VLOOKUP(D4,assignees!$F$6:$G$8,2,0)</f>
+        <v>G2</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f>VLOOKUP(E4,assignees!$G$2:$H$4,2,0)</f>
+        <v>jclarkeSTFC, warunawickramasingha, SilkeSchomann, adriazalvarez</v>
+      </c>
+      <c r="G4" s="2">
         <f t="shared" si="0"/>
         <v>124.2</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>111</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>120</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>150</v>
-      </c>
-      <c r="J4" s="1">
-        <v>120</v>
       </c>
       <c r="K4" s="1">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="1" t="str">
-        <f>VLOOKUP(D5,assignees!$G$2:$H$4,2,0)</f>
-        <v>MohamedAlmaki, MialLewis, sf1919</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="D5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="str">
+        <f>VLOOKUP(D5,assignees!$F$6:$G$8,2,0)</f>
+        <v>G2</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f>VLOOKUP(E5,assignees!$G$2:$H$4,2,0)</f>
+        <v>jclarkeSTFC, warunawickramasingha, SilkeSchomann, adriazalvarez</v>
+      </c>
+      <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>77.5</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>120</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>85</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>45</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1399,63 +1430,71 @@
         <v>25</v>
       </c>
       <c r="C6"/>
-      <c r="D6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="1" t="str">
-        <f>VLOOKUP(D6,assignees!$G$2:$H$4,2,0)</f>
-        <v>SilkeSchomann, warunawickramasingha, jclarkeSTFC, adriazalvarez</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="D6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" t="str">
+        <f>VLOOKUP(D6,assignees!$F$6:$G$8,2,0)</f>
+        <v>G3</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f>VLOOKUP(E6,assignees!$G$2:$H$4,2,0)</f>
+        <v>MohamedAlmaki, cailafinn, GuiMacielPereira, RichardWaiteSTFC</v>
+      </c>
+      <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>60</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>105</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>90</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>60</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7"/>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="1" t="str">
-        <f>VLOOKUP(D7,assignees!$G$2:$H$4,2,0)</f>
-        <v xml:space="preserve">GuiMacielPereira, jhaigh0, cailafinn, thomashampson </v>
-      </c>
-      <c r="F7" s="2">
+      <c r="D7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" t="str">
+        <f>VLOOKUP(D7,assignees!$F$6:$G$8,2,0)</f>
+        <v>G1</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f>VLOOKUP(E7,assignees!$G$2:$H$4,2,0)</f>
+        <v>jhaigh0, MialLewis, thomashampson, andy-bridger</v>
+      </c>
+      <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>86.666666666666671</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>30</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>110</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1463,31 +1502,35 @@
         <v>32</v>
       </c>
       <c r="C8"/>
-      <c r="D8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="1" t="str">
-        <f>VLOOKUP(D8,assignees!$G$2:$H$4,2,0)</f>
-        <v xml:space="preserve">GuiMacielPereira, jhaigh0, cailafinn, thomashampson </v>
-      </c>
-      <c r="F8" s="2">
+      <c r="D8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" t="str">
+        <f>VLOOKUP(D8,assignees!$F$6:$G$8,2,0)</f>
+        <v>G1</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <f>VLOOKUP(E8,assignees!$G$2:$H$4,2,0)</f>
+        <v>jhaigh0, MialLewis, thomashampson, andy-bridger</v>
+      </c>
+      <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>71.25</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>67</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>53</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>70</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1495,96 +1538,108 @@
         <v>38</v>
       </c>
       <c r="C9"/>
-      <c r="D9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="1" t="str">
-        <f>VLOOKUP(D9,assignees!$G$2:$H$4,2,0)</f>
-        <v>SilkeSchomann, warunawickramasingha, jclarkeSTFC, adriazalvarez</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="D9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" t="str">
+        <f>VLOOKUP(D9,assignees!$F$6:$G$8,2,0)</f>
+        <v>G3</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <f>VLOOKUP(E9,assignees!$G$2:$H$4,2,0)</f>
+        <v>MohamedAlmaki, cailafinn, GuiMacielPereira, RichardWaiteSTFC</v>
+      </c>
+      <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>59.25</v>
       </c>
-      <c r="G9" s="1">
-        <v>60</v>
-      </c>
       <c r="H9" s="1">
         <v>60</v>
       </c>
       <c r="I9" s="1">
+        <v>60</v>
+      </c>
+      <c r="J9" s="1">
         <v>50</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="1" t="str">
-        <f>VLOOKUP(D10,assignees!$G$2:$H$4,2,0)</f>
-        <v>MohamedAlmaki, MialLewis, sf1919</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="D10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" t="str">
+        <f>VLOOKUP(D10,assignees!$F$6:$G$8,2,0)</f>
+        <v>G2</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <f>VLOOKUP(E10,assignees!$G$2:$H$4,2,0)</f>
+        <v>jclarkeSTFC, warunawickramasingha, SilkeSchomann, adriazalvarez</v>
+      </c>
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>60</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>40</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>60</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="1" t="str">
-        <f>VLOOKUP(D11,assignees!$G$2:$H$4,2,0)</f>
-        <v>MohamedAlmaki, MialLewis, sf1919</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="D11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" t="str">
+        <f>VLOOKUP(D11,assignees!$F$6:$G$8,2,0)</f>
+        <v>G2</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f>VLOOKUP(E11,assignees!$G$2:$H$4,2,0)</f>
+        <v>jclarkeSTFC, warunawickramasingha, SilkeSchomann, adriazalvarez</v>
+      </c>
+      <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>38.799999999999997</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>50</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>30</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>36</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>45</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1592,100 +1647,112 @@
         <v>24</v>
       </c>
       <c r="C12"/>
-      <c r="D12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="1" t="str">
-        <f>VLOOKUP(D12,assignees!$G$2:$H$4,2,0)</f>
-        <v>SilkeSchomann, warunawickramasingha, jclarkeSTFC, adriazalvarez</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="D12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="str">
+        <f>VLOOKUP(D12,assignees!$F$6:$G$8,2,0)</f>
+        <v>G3</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f>VLOOKUP(E12,assignees!$G$2:$H$4,2,0)</f>
+        <v>MohamedAlmaki, cailafinn, GuiMacielPereira, RichardWaiteSTFC</v>
+      </c>
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
         <v>27.2</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>22</v>
-      </c>
-      <c r="H12" s="1">
-        <v>20</v>
       </c>
       <c r="I12" s="1">
         <v>20</v>
       </c>
       <c r="J12" s="1">
+        <v>20</v>
+      </c>
+      <c r="K12" s="1">
         <v>44</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L12" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="1" t="str">
-        <f>VLOOKUP(D13,assignees!$G$2:$H$4,2,0)</f>
-        <v>SilkeSchomann, warunawickramasingha, jclarkeSTFC, adriazalvarez</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="D13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="str">
+        <f>VLOOKUP(D13,assignees!$F$6:$G$8,2,0)</f>
+        <v>G3</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <f>VLOOKUP(E13,assignees!$G$2:$H$4,2,0)</f>
+        <v>MohamedAlmaki, cailafinn, GuiMacielPereira, RichardWaiteSTFC</v>
+      </c>
+      <c r="G13" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>26</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>20</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>30</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14"/>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="1" t="str">
-        <f>VLOOKUP(D14,assignees!$G$2:$H$4,2,0)</f>
-        <v xml:space="preserve">GuiMacielPereira, jhaigh0, cailafinn, thomashampson </v>
-      </c>
-      <c r="F14" s="2">
+      <c r="D14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="str">
+        <f>VLOOKUP(D14,assignees!$F$6:$G$8,2,0)</f>
+        <v>G1</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f>VLOOKUP(E14,assignees!$G$2:$H$4,2,0)</f>
+        <v>jhaigh0, MialLewis, thomashampson, andy-bridger</v>
+      </c>
+      <c r="G14" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>11</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>0</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>45</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <v>15</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1693,154 +1760,171 @@
         <v>22</v>
       </c>
       <c r="C15"/>
-      <c r="D15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="1" t="str">
-        <f>VLOOKUP(D15,assignees!$G$2:$H$4,2,0)</f>
-        <v>SilkeSchomann, warunawickramasingha, jclarkeSTFC, adriazalvarez</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="D15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" t="str">
+        <f>VLOOKUP(D15,assignees!$F$6:$G$8,2,0)</f>
+        <v>G3</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <f>VLOOKUP(E15,assignees!$G$2:$H$4,2,0)</f>
+        <v>MohamedAlmaki, cailafinn, GuiMacielPereira, RichardWaiteSTFC</v>
+      </c>
+      <c r="G15" s="2">
         <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>20</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>0</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="1" t="str">
-        <f>VLOOKUP(D16,assignees!$G$2:$H$4,2,0)</f>
-        <v>MohamedAlmaki, MialLewis, sf1919</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="D16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="str">
+        <f>VLOOKUP(D16,assignees!$F$6:$G$8,2,0)</f>
+        <v>G2</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <f>VLOOKUP(E16,assignees!$G$2:$H$4,2,0)</f>
+        <v>jclarkeSTFC, warunawickramasingha, SilkeSchomann, adriazalvarez</v>
+      </c>
+      <c r="G16" s="2">
         <f t="shared" si="0"/>
         <v>17.600000000000001</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>25</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>10</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>20</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <v>21</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17"/>
-      <c r="D17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="1" t="str">
-        <f>VLOOKUP(D17,assignees!$G$2:$H$4,2,0)</f>
-        <v>MohamedAlmaki, MialLewis, sf1919</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="D17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" t="str">
+        <f>VLOOKUP(D17,assignees!$F$6:$G$8,2,0)</f>
+        <v>G2</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <f>VLOOKUP(E17,assignees!$G$2:$H$4,2,0)</f>
+        <v>jclarkeSTFC, warunawickramasingha, SilkeSchomann, adriazalvarez</v>
+      </c>
+      <c r="G17" s="2">
         <f t="shared" si="0"/>
         <v>18.600000000000001</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>15</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>30</v>
-      </c>
-      <c r="I17" s="1">
-        <v>15</v>
       </c>
       <c r="J17" s="1">
         <v>15</v>
       </c>
       <c r="K17" s="1">
+        <v>15</v>
+      </c>
+      <c r="L17" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="1" t="str">
-        <f>VLOOKUP(D18,assignees!$G$2:$H$4,2,0)</f>
-        <v>SilkeSchomann, warunawickramasingha, jclarkeSTFC, adriazalvarez</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="D18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" t="str">
+        <f>VLOOKUP(D18,assignees!$F$6:$G$8,2,0)</f>
+        <v>G3</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f>VLOOKUP(E18,assignees!$G$2:$H$4,2,0)</f>
+        <v>MohamedAlmaki, cailafinn, GuiMacielPereira, RichardWaiteSTFC</v>
+      </c>
+      <c r="G18" s="2">
         <f t="shared" si="0"/>
         <v>14.4</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>10</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>20</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>17</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K18" s="1">
         <v>15</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L18" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="1" t="str">
-        <f>VLOOKUP(D19,assignees!$G$2:$H$4,2,0)</f>
-        <v xml:space="preserve">GuiMacielPereira, jhaigh0, cailafinn, thomashampson </v>
-      </c>
-      <c r="F19" s="2">
+      <c r="D19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" t="str">
+        <f>VLOOKUP(D19,assignees!$F$6:$G$8,2,0)</f>
+        <v>G1</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <f>VLOOKUP(E19,assignees!$G$2:$H$4,2,0)</f>
+        <v>jhaigh0, MialLewis, thomashampson, andy-bridger</v>
+      </c>
+      <c r="G19" s="2">
         <f t="shared" si="0"/>
         <v>13.75</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>10</v>
-      </c>
-      <c r="I19" s="1">
-        <v>15</v>
       </c>
       <c r="J19" s="1">
         <v>15</v>
@@ -1848,8 +1932,11 @@
       <c r="K19" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L19" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1857,50 +1944,55 @@
         <v>27</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="1" t="str">
-        <f>VLOOKUP(D20,assignees!$G$2:$H$4,2,0)</f>
-        <v xml:space="preserve">GuiMacielPereira, jhaigh0, cailafinn, thomashampson </v>
-      </c>
-      <c r="F20" s="2">
+      <c r="D20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" t="str">
+        <f>VLOOKUP(D20,assignees!$F$6:$G$8,2,0)</f>
+        <v>G1</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <f>VLOOKUP(E20,assignees!$G$2:$H$4,2,0)</f>
+        <v>jhaigh0, MialLewis, thomashampson, andy-bridger</v>
+      </c>
+      <c r="G20" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>10</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>15</v>
       </c>
-      <c r="J20" s="1">
+      <c r="K20" s="1">
         <v>10</v>
       </c>
-      <c r="K20" s="1">
+      <c r="L20" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C21" s="11"/>
-      <c r="D21" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="11" t="str">
-        <f>VLOOKUP(D21,assignees!$G$2:$H$4,2,0)</f>
-        <v xml:space="preserve">GuiMacielPereira, jhaigh0, cailafinn, thomashampson </v>
-      </c>
-      <c r="F21" s="11">
+      <c r="D21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" t="str">
+        <f>VLOOKUP(D21,assignees!$F$6:$G$8,2,0)</f>
+        <v>G1</v>
+      </c>
+      <c r="F21" s="11" t="str">
+        <f>VLOOKUP(E21,assignees!$G$2:$H$4,2,0)</f>
+        <v>jhaigh0, MialLewis, thomashampson, andy-bridger</v>
+      </c>
+      <c r="G21" s="11">
         <v>20</v>
-      </c>
-      <c r="G21" s="11">
-        <v>0</v>
       </c>
       <c r="H21" s="11">
         <v>0</v>
@@ -1914,27 +2006,31 @@
       <c r="K21" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="L21" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C22" s="11"/>
-      <c r="D22" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="11" t="str">
-        <f>VLOOKUP(D22,assignees!$G$2:$H$4,2,0)</f>
-        <v>SilkeSchomann, warunawickramasingha, jclarkeSTFC, adriazalvarez</v>
-      </c>
-      <c r="F22" s="11">
+      <c r="D22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" t="str">
+        <f>VLOOKUP(D22,assignees!$F$6:$G$8,2,0)</f>
+        <v>G3</v>
+      </c>
+      <c r="F22" s="11" t="str">
+        <f>VLOOKUP(E22,assignees!$G$2:$H$4,2,0)</f>
+        <v>MohamedAlmaki, cailafinn, GuiMacielPereira, RichardWaiteSTFC</v>
+      </c>
+      <c r="G22" s="11">
         <v>20</v>
-      </c>
-      <c r="G22" s="11">
-        <v>0</v>
       </c>
       <c r="H22" s="11">
         <v>0</v>
@@ -1948,27 +2044,31 @@
       <c r="K22" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="L22" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C23" s="11"/>
-      <c r="D23" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="11" t="str">
-        <f>VLOOKUP(D23,assignees!$G$2:$H$4,2,0)</f>
-        <v>MohamedAlmaki, MialLewis, sf1919</v>
-      </c>
-      <c r="F23" s="11">
+      <c r="D23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="str">
+        <f>VLOOKUP(D23,assignees!$F$6:$G$8,2,0)</f>
+        <v>G2</v>
+      </c>
+      <c r="F23" s="11" t="str">
+        <f>VLOOKUP(E23,assignees!$G$2:$H$4,2,0)</f>
+        <v>jclarkeSTFC, warunawickramasingha, SilkeSchomann, adriazalvarez</v>
+      </c>
+      <c r="G23" s="11">
         <v>20</v>
-      </c>
-      <c r="G23" s="11">
-        <v>0</v>
       </c>
       <c r="H23" s="11">
         <v>0</v>
@@ -1982,11 +2082,14 @@
       <c r="K23" s="11">
         <v>0</v>
       </c>
+      <c r="L23" s="11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K20" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K20">
-      <sortCondition descending="1" ref="F1:F20"/>
+  <autoFilter ref="A1:L20" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L20">
+      <sortCondition descending="1" ref="G1:G20"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="22" type="noConversion"/>
@@ -2012,7 +2115,7 @@
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C19:C24 D24</xm:sqref>
+          <xm:sqref>C19:C24 D24:E24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -2020,9 +2123,9 @@
           </x14:formula1>
           <xm:sqref>C2:C18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1CDE1CA9-DBC2-4449-8ED0-EBB9612B23D5}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{01DB916E-D503-464C-949D-E79C78412D40}">
           <x14:formula1>
-            <xm:f>assignees!$G$2:$G$4</xm:f>
+            <xm:f>assignees!$F$6:$F$8</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D23</xm:sqref>
         </x14:dataValidation>
@@ -2037,7 +2140,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2045,7 +2148,7 @@
     <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="81.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" customWidth="1"/>
     <col min="8" max="8" width="63.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
@@ -2058,14 +2161,14 @@
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>76</v>
+      <c r="F1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
@@ -2073,17 +2176,17 @@
         <v>39</v>
       </c>
       <c r="B2">
-        <f>COUNTIF(issues!$E$2:$E$20,"*"&amp;A2&amp;"*")</f>
-        <v>6</v>
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A2&amp;"*")</f>
+        <v>7</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
@@ -2091,16 +2194,16 @@
         <v>40</v>
       </c>
       <c r="B3">
-        <f>COUNTIF(issues!$E$2:$E$20,"*"&amp;A3&amp;"*")</f>
-        <v>6</v>
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A3&amp;"*")</f>
+        <v>7</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2109,16 +2212,16 @@
         <v>41</v>
       </c>
       <c r="B4">
-        <f>COUNTIF(issues!$E$2:$E$20,"*"&amp;A4&amp;"*")</f>
-        <v>7</v>
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A4&amp;"*")</f>
+        <v>6</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2127,8 +2230,8 @@
         <v>42</v>
       </c>
       <c r="B5">
-        <f>COUNTIF(issues!$E$2:$E$20,"*"&amp;A5&amp;"*")</f>
-        <v>7</v>
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A5&amp;"*")</f>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -2136,35 +2239,54 @@
         <v>43</v>
       </c>
       <c r="B6">
-        <f>COUNTIF(issues!$E$2:$E$20,"*"&amp;A6&amp;"*")</f>
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A6&amp;"*")</f>
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7">
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A7&amp;"*")</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7">
-        <f>COUNTIF(issues!$E$2:$E$20,"*"&amp;#REF!&amp;"*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>44</v>
       </c>
       <c r="B8">
-        <f>COUNTIF(issues!$E$2:$E$20,"*"&amp;A8&amp;"*")</f>
-        <v>7</v>
-      </c>
-      <c r="G8" s="1"/>
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A8&amp;"*")</f>
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>45</v>
       </c>
       <c r="B9">
-        <f>COUNTIF(issues!$E$2:$E$20,"*"&amp;A9&amp;"*")</f>
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A9&amp;"*")</f>
         <v>6</v>
       </c>
     </row>
@@ -2173,31 +2295,35 @@
         <v>46</v>
       </c>
       <c r="B10">
-        <f>COUNTIF(issues!$E$2:$E$20,"*"&amp;A10&amp;"*")</f>
-        <v>7</v>
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A10&amp;"*")</f>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B11">
-        <f>COUNTIF(issues!$E$2:$E$20,"*"&amp;A11&amp;"*")</f>
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A11&amp;"*")</f>
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>56</v>
+      <c r="A12" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="B12">
-        <f>COUNTIF(issues!$E$2:$E$20,"*"&amp;#REF!&amp;"*")</f>
-        <v>0</v>
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A12&amp;"*")</f>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>61</v>
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13">
+        <f>COUNTIF(issues!$F$2:$F$20,"*"&amp;A13&amp;"*")</f>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="6:13" x14ac:dyDescent="0.3">
@@ -2272,7 +2398,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C12">
     <sortCondition descending="1" ref="B3:B23"/>
   </sortState>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B15:B1048576 B1:B13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>